<commit_message>
Complied report into one page document - convert to pdf for submission
</commit_message>
<xml_diff>
--- a/reports/Data & Graphs.xlsx
+++ b/reports/Data & Graphs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\web\blackjack\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\uni\241\week09\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8415" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8415" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data - Uniform Shuffle" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Distribution of Unbroken Pairs when Shuffling a 50 Card Deck Uniformly</a:t>
+              <a:t>Unbroken Pair Distribution with Random Permutations</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -584,6 +584,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -615,11 +616,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -659,29 +660,13 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:name>Trendline</c:name>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'Data - One Random Shuffle'!$A$3:$A$19</c:f>
@@ -816,8 +801,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="415865400"/>
         <c:axId val="415867368"/>
       </c:barChart>
@@ -828,6 +813,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> of Unbroken Pairs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -853,8 +898,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -894,6 +939,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>RATIO</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -913,8 +1013,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -937,37 +1037,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -997,6 +1066,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1415,6 +1485,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2064,509 +2135,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3091,11 +2659,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart1"/>
   <sheetViews>
-    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3106,7 +3199,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3117,7 +3210,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3128,7 +3221,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6090000"/>
+    <xdr:ext cx="9304299" cy="6075091"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3158,10 +3251,64 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.95379</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.23061</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90CEAD6F-E159-4E4F-854F-E4E2C2F6C977}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="5794354"/>
+          <a:ext cx="2145632" cy="280737"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(sample size = 1,000,000)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6090000"/>
+    <xdr:ext cx="9294395" cy="6075947"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3190,11 +3337,128 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.9538</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.17476</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F450C3-0537-4581-BDB5-39FAF4FB3622}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="5805236"/>
+          <a:ext cx="1624263" cy="280737"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(sample size = 100,000)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6090000"/>
+    <xdr:ext cx="9294395" cy="6075947"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3221,6 +3485,123 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.9538</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.17476</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668D659E-5571-4134-A8B7-F0102C7CE5C5}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="5795210"/>
+          <a:ext cx="1624263" cy="280737"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(sample size = 100,000)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3642,7 +4023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>